<commit_message>
upd yeast growth data
</commit_message>
<xml_diff>
--- a/data/LA_yeast_growth.xlsx
+++ b/data/LA_yeast_growth.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1681971665" val="1050" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1681971665" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1681971665"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1681971665"/>
+      <pm:revision xmlns:pm="smNativeData" day="1691498225" val="1050" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1691498225" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1691498225" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1691498225"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="24">
   <si>
     <t>sample_id</t>
   </si>
@@ -49,25 +49,28 @@
     <t>RGR</t>
   </si>
   <si>
+    <t>RGR2</t>
+  </si>
+  <si>
     <t>20220720_2</t>
   </si>
   <si>
     <t>control</t>
   </si>
   <si>
-    <t>DL0005</t>
-  </si>
-  <si>
-    <t>DL0050</t>
-  </si>
-  <si>
-    <t>DL0500</t>
-  </si>
-  <si>
-    <t>DL4500</t>
-  </si>
-  <si>
-    <t>LL4500</t>
+    <t>DLA0005</t>
+  </si>
+  <si>
+    <t>DLA0050</t>
+  </si>
+  <si>
+    <t>DLA0500</t>
+  </si>
+  <si>
+    <t>DLA4500</t>
+  </si>
+  <si>
+    <t>LLA4500</t>
   </si>
   <si>
     <t>20220720_3</t>
@@ -86,6 +89,12 @@
   </si>
   <si>
     <t>20230301_1</t>
+  </si>
+  <si>
+    <t>20230808_0</t>
+  </si>
+  <si>
+    <t>DLS4500</t>
   </si>
 </sst>
 </file>
@@ -110,7 +119,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1681971665" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1691498225" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -125,7 +134,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1681971665" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1691498225" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
@@ -147,7 +156,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1681971665" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1691498225" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -169,7 +178,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681971665"/>
+          <pm:border xmlns:pm="smNativeData" id="1691498225"/>
         </ext>
       </extLst>
     </border>
@@ -188,7 +197,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1681971665"/>
+          <pm:border xmlns:pm="smNativeData" id="1691498225"/>
         </ext>
       </extLst>
     </border>
@@ -205,7 +214,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1681971665" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1691498225" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -469,10 +478,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H43"/>
+  <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H43"/>
+    <sheetView tabSelected="1" view="normal" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="13.45"/>
@@ -482,7 +491,7 @@
     <col min="7" max="7" width="16.297297" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -507,13 +516,16 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2">
         <f>0.559*2.9/3</f>
@@ -538,13 +550,17 @@
         <f>(LN(D2)-LN(C2))/E2</f>
         <v>0.260422819957922158</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <f>(LOG(D2,2)-LOG(C2,2))/E2</f>
+        <v>0.375710710887612809</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <f>0.559*2.9/3</f>
@@ -569,13 +585,17 @@
         <f>(LN(D3)-LN(C3))/E3</f>
         <v>0.28694416726273948</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <f>(LOG(D3,2)-LOG(C3,2))/E3</f>
+        <v>0.413972927121965828</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <f>0.559*2.9/3</f>
@@ -600,13 +620,17 @@
         <f>(LN(D4)-LN(C4))/E4</f>
         <v>0.210425520593956872</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <f>(LOG(D4,2)-LOG(C4,2))/E4</f>
+        <v>0.303579855037381208</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5">
         <f>0.559*2.9/3</f>
@@ -631,13 +655,17 @@
         <f>(LN(D5)-LN(C5))/E5</f>
         <v>0.139972768156785477</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <f>(LOG(D5,2)-LOG(C5,2))/E5</f>
+        <v>0.201938018479294934</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <f>0.559*2.9/3</f>
@@ -662,13 +690,17 @@
         <f>(LN(D6)-LN(C6))/E6</f>
         <v>0.0109170146123322521</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <f>(LOG(D6,2)-LOG(C6,2))/E6</f>
+        <v>0.015749922842524045</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7">
         <f>0.559*2.9/3</f>
@@ -693,13 +725,17 @@
         <f>(LN(D7)-LN(C7))/E7</f>
         <v>0.0239982234087996238</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <f>(LOG(D7,2)-LOG(C7,2))/E7</f>
+        <v>0.0346221179020207703</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C8">
         <f>0.611*2.9/3</f>
@@ -724,13 +760,17 @@
         <f>(LN(D8)-LN(C8))/E8</f>
         <v>0.191908400386168054</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <f>(LOG(D8,2)-LOG(C8,2))/E8</f>
+        <v>0.276865297542059086</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9">
         <f>0.611*2.9/3</f>
@@ -755,13 +795,17 @@
         <f>(LN(D9)-LN(C9))/E9</f>
         <v>0.127018308013192582</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <f>(LOG(D9,2)-LOG(C9,2))/E9</f>
+        <v>0.18324868307273988</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <f>0.611*2.9/3</f>
@@ -784,22 +828,26 @@
       </c>
       <c r="H10">
         <f>(LN(D10)-LN(C10))/E10</f>
-        <v>0.108439886616976455</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
+        <v>0.108439886616976722</v>
+      </c>
+      <c r="I10">
+        <f>(LOG(D10,2)-LOG(C10,2))/E10</f>
+        <v>0.156445686656873661</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11">
         <f>0.611*2.9/3</f>
         <v>0.590633333333333344</v>
       </c>
       <c r="D11" t="n">
-        <v>0.825999999999999979</v>
+        <v>0.825999999999999801</v>
       </c>
       <c r="E11">
         <f>14+25/60-10-4/6</f>
@@ -817,13 +865,17 @@
         <f>(LN(D11)-LN(C11))/E11</f>
         <v>0.0894398309400163427</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <f>(LOG(D11,2)-LOG(C11,2))/E11</f>
+        <v>0.129034400555108842</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <f>0.611*2.9/3</f>
@@ -848,13 +900,17 @@
         <f>(LN(D12)-LN(C12))/E12</f>
         <v>0.0112137482766948438</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <f>(LOG(D12,2)-LOG(C12,2))/E12</f>
+        <v>0.0161780190285646697</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
         <v>15</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
       </c>
       <c r="C13">
         <f>0.611*2.9/3</f>
@@ -879,13 +935,17 @@
         <f>(LN(D13)-LN(C13))/E13</f>
         <v>0.000616327303491195089</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <f>(LOG(D13,2)-LOG(C13,2))/E13</f>
+        <v>0.000889172344310926199</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C14">
         <f>0.541*2.9/3</f>
@@ -910,13 +970,17 @@
         <f>(LN(D14)-LN(C14))/E14</f>
         <v>0.26141904479783058</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <f>(LOG(D14,2)-LOG(C14,2))/E14</f>
+        <v>0.377147959523761278</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15">
         <f>0.541*2.9/3</f>
@@ -941,13 +1005,17 @@
         <f>(LN(D15)-LN(C15))/E15</f>
         <v>0.284262233670575082</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <f>(LOG(D15,2)-LOG(C15,2))/E15</f>
+        <v>0.410103714828556942</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C16">
         <f>0.541*2.9/3</f>
@@ -972,13 +1040,17 @@
         <f>(LN(D16)-LN(C16))/E16</f>
         <v>0.281815734381423688</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <f>(LOG(D16,2)-LOG(C16,2))/E16</f>
+        <v>0.406574162436562503</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C17">
         <f>0.541*2.9/3</f>
@@ -1003,13 +1075,17 @@
         <f>(LN(D17)-LN(C17))/E17</f>
         <v>0.218788604851967117</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <f>(LOG(D17,2)-LOG(C17,2))/E17</f>
+        <v>0.315645235222948717</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <f>0.541*2.9/3</f>
@@ -1034,13 +1110,17 @@
         <f>(LN(D18)-LN(C18))/E18</f>
         <v>0.100699442432245689</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <f>(LOG(D18,2)-LOG(C18,2))/E18</f>
+        <v>0.145278586217284333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19">
         <f>0.541*2.9/3</f>
@@ -1065,13 +1145,17 @@
         <f>(LN(D19)-LN(C19))/E19</f>
         <v>0.0973944471216776897</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <f>(LOG(D19,2)-LOG(C19,2))/E19</f>
+        <v>0.140510485872566875</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20">
         <f>1.032*1.5/3</f>
@@ -1095,13 +1179,17 @@
         <f>(LN(D20)-LN(C20))/E20</f>
         <v>0.302575678699093364</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <f>(LOG(D20,2)-LOG(C20,2))/E20</f>
+        <v>0.436524431152793291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C21">
         <f>1.032*1.5/3</f>
@@ -1125,13 +1213,17 @@
         <f>(LN(D21)-LN(C21))/E21</f>
         <v>0.284089624369741323</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <f>(LOG(D21,2)-LOG(C21,2))/E21</f>
+        <v>0.409854692246233299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C22">
         <f>1.032*1.5/3</f>
@@ -1155,13 +1247,17 @@
         <f>(LN(D22)-LN(C22))/E22</f>
         <v>0.279652509490327983</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <f>(LOG(D22,2)-LOG(C22,2))/E22</f>
+        <v>0.403453288613849992</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C23">
         <f>1.032*1.5/3</f>
@@ -1185,13 +1281,17 @@
         <f>(LN(D23)-LN(C23))/E23</f>
         <v>0.219213497367678345</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <f>(LOG(D23,2)-LOG(C23,2))/E23</f>
+        <v>0.316258225548275629</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C24">
         <f>1.032*1.5/3</f>
@@ -1215,13 +1315,17 @@
         <f>(LN(D24)-LN(C24))/E24</f>
         <v>0.167550927336705318</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24">
+        <f>(LOG(D24,2)-LOG(C24,2))/E24</f>
+        <v>0.241724891965012034</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25">
         <f>1.032*1.5/3</f>
@@ -1245,13 +1349,17 @@
         <f>(LN(D25)-LN(C25))/E25</f>
         <v>0.27656736616560802</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25">
+        <f>(LOG(D25,2)-LOG(C25,2))/E25</f>
+        <v>0.399002367638843261</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B26" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C26">
         <f>0.926*1.5/3</f>
@@ -1275,13 +1383,17 @@
         <f>(LN(D26)-LN(C26))/E26</f>
         <v>0.397122227386786655</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26">
+        <f>(LOG(D26,2)-LOG(C26,2))/E26</f>
+        <v>0.572926268077696665</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B27" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C27">
         <f>0.926*1.5/3</f>
@@ -1305,13 +1417,17 @@
         <f>(LN(D27)-LN(C27))/E27</f>
         <v>0.410624555480059961</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27">
+        <f>(LOG(D27,2)-LOG(C27,2))/E27</f>
+        <v>0.592406009858316729</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B28" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C28">
         <f>0.926*1.5/3</f>
@@ -1335,20 +1451,24 @@
         <f>(LN(D28)-LN(C28))/E28</f>
         <v>0.381219536494683311</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28">
+        <f>(LOG(D28,2)-LOG(C28,2))/E28</f>
+        <v>0.549983534790866724</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B29" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C29">
         <f>0.926*1.5/3</f>
         <v>0.462999999999999989</v>
       </c>
       <c r="D29" t="n">
-        <v>1.11299999999999999</v>
+        <v>1.11300000000000021</v>
       </c>
       <c r="E29" t="n">
         <v>3</v>
@@ -1365,13 +1485,17 @@
         <f>(LN(D29)-LN(C29))/E29</f>
         <v>0.292362432396437022</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29">
+        <f>(LOG(D29,2)-LOG(C29,2))/E29</f>
+        <v>0.421789831360573331</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <f>0.926*1.5/3</f>
@@ -1395,13 +1519,17 @@
         <f>(LN(D30)-LN(C30))/E30</f>
         <v>0.26685247664357532</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30">
+        <f>(LOG(D30,2)-LOG(C30,2))/E30</f>
+        <v>0.384986744702623351</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B31" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C31">
         <f>0.926*1.5/3</f>
@@ -1425,13 +1553,17 @@
         <f>(LN(D31)-LN(C31))/E31</f>
         <v>0.317727589331250027</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31">
+        <f>(LOG(D31,2)-LOG(C31,2))/E31</f>
+        <v>0.458384017481799955</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C32">
         <f>0.894*1.5/3</f>
@@ -1455,13 +1587,17 @@
         <f>(LN(D32)-LN(C32))/E32</f>
         <v>0.357388571740936634</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32">
+        <f>(LOG(D32,2)-LOG(C32,2))/E32</f>
+        <v>0.515602720121036739</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C33">
         <f>0.894*1.5/3</f>
@@ -1485,13 +1621,17 @@
         <f>(LN(D33)-LN(C33))/E33</f>
         <v>0.336317840627530007</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33">
+        <f>(LOG(D33,2)-LOG(C33,2))/E33</f>
+        <v>0.485204080835823337</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B34" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C34">
         <f>0.894*1.5/3</f>
@@ -1515,13 +1655,17 @@
         <f>(LN(D34)-LN(C34))/E34</f>
         <v>0.328616728020608662</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34">
+        <f>(LOG(D34,2)-LOG(C34,2))/E34</f>
+        <v>0.474093723868490002</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B35" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C35">
         <f>0.894*1.5/3</f>
@@ -1545,13 +1689,17 @@
         <f>(LN(D35)-LN(C35))/E35</f>
         <v>0.264711912336380983</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35">
+        <f>(LOG(D35,2)-LOG(C35,2))/E35</f>
+        <v>0.381898563191930016</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B36" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C36">
         <f>0.894*1.5/3</f>
@@ -1575,13 +1723,17 @@
         <f>(LN(D36)-LN(C36))/E36</f>
         <v>0.286245817098865984</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36">
+        <f>(LOG(D36,2)-LOG(C36,2))/E36</f>
+        <v>0.412965420803743388</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C37">
         <f>0.894*1.5/3</f>
@@ -1605,13 +1757,17 @@
         <f>(LN(D37)-LN(C37))/E37</f>
         <v>0.336317840627530007</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37">
+        <f>(LOG(D37,2)-LOG(C37,2))/E37</f>
+        <v>0.485204080835823337</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B38" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C38" t="n">
         <v>0.366000000000000014</v>
@@ -1634,13 +1790,17 @@
         <f>(LN(D38)-LN(C38))/E38</f>
         <v>0.347472576774823283</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38">
+        <f>(LOG(D38,2)-LOG(C38,2))/E38</f>
+        <v>0.501296963357943248</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B39" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C39" t="n">
         <v>0.310999999999999988</v>
@@ -1663,13 +1823,17 @@
         <f>(LN(D39)-LN(C39))/E39</f>
         <v>0.317016455079775339</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39">
+        <f>(LOG(D39,2)-LOG(C39,2))/E39</f>
+        <v>0.45735806762379001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B40" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C40" t="n">
         <v>0.227000000000000002</v>
@@ -1692,13 +1856,17 @@
         <f>(LN(D40)-LN(C40))/E40</f>
         <v>0.405410717419726652</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40">
+        <f>(LOG(D40,2)-LOG(C40,2))/E40</f>
+        <v>0.584884031544680028</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B41" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C41" t="n">
         <v>0.45</v>
@@ -1721,13 +1889,17 @@
         <f>(LN(D41)-LN(C41))/E41</f>
         <v>0.190535698675283331</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41">
+        <f>(LOG(D41,2)-LOG(C41,2))/E41</f>
+        <v>0.274884907591144989</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B42" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C42" t="n">
         <v>0.533999999999999986</v>
@@ -1750,13 +1922,17 @@
         <f>(LN(D42)-LN(C42))/E42</f>
         <v>0.00310657731626733336</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42">
+        <f>(LOG(D42,2)-LOG(C42,2))/E42</f>
+        <v>0.00448184368831699942</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C43" t="n">
         <v>0.408000000000000007</v>
@@ -1778,13 +1954,119 @@
       <c r="H43">
         <f>(LN(D43)-LN(C43))/E43</f>
         <v>0.135699253844016687</v>
+      </c>
+      <c r="I43">
+        <f>(LOG(D43,2)-LOG(C43,2))/E43</f>
+        <v>0.195772640573094652</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" t="n">
+        <v>0.433000000000000007</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1.03699999999999992</v>
+      </c>
+      <c r="E44">
+        <f>3+35/60</f>
+        <v>3.58333333333333304</v>
+      </c>
+      <c r="F44">
+        <f>LOG(D44/C44)</f>
+        <v>0.37929086003567547</v>
+      </c>
+      <c r="G44">
+        <f>E44*LOG(2)/F44</f>
+        <v>2.84396733866581606</v>
+      </c>
+      <c r="H44">
+        <f>(LN(D44)-LN(C44))/E44</f>
+        <v>0.24372543634242918</v>
+      </c>
+      <c r="I44">
+        <f>(LOG(D44,2)-LOG(C44,2))/E44</f>
+        <v>0.351621478349721261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.436000000000000032</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.837999999999999901</v>
+      </c>
+      <c r="E45">
+        <f>3+35/60</f>
+        <v>3.58333333333333304</v>
+      </c>
+      <c r="F45">
+        <f>LOG(D45/C45)</f>
+        <v>0.283757529361690466</v>
+      </c>
+      <c r="G45">
+        <f>E45*LOG(2)/F45</f>
+        <v>3.80145267060377723</v>
+      </c>
+      <c r="H45">
+        <f>(LN(D45)-LN(C45))/E45</f>
+        <v>0.182337448502246424</v>
+      </c>
+      <c r="I45">
+        <f>(LOG(D45,2)-LOG(C45,2))/E45</f>
+        <v>0.263057332722537174</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" t="n">
+        <v>0.527000000000000046</v>
+      </c>
+      <c r="D46" t="n">
+        <v>1.21100000000000008</v>
+      </c>
+      <c r="E46">
+        <f>3+35/60</f>
+        <v>3.58333333333333304</v>
+      </c>
+      <c r="F46">
+        <f>LOG(D46/C46)</f>
+        <v>0.361333527930505616</v>
+      </c>
+      <c r="G46">
+        <f>E46*LOG(2)/F46</f>
+        <v>2.98530508357195892</v>
+      </c>
+      <c r="H46">
+        <f>(LN(D46)-LN(C46))/E46</f>
+        <v>0.232186380003273696</v>
+      </c>
+      <c r="I46">
+        <f>(LOG(D46,2)-LOG(C46,2))/E46</f>
+        <v>0.334974138992685022</v>
       </c>
     </row>
   </sheetData>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1681971665" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1691498225" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -1793,14 +2075,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1681971665" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1681971665" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1691498225" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1691498225" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1681971665" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1691498225" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>